<commit_message>
Adding tp_1123 test script. and changed password
</commit_message>
<xml_diff>
--- a/src/main/resources/Reference Ranges Iron 21042023DP.xlsx
+++ b/src/main/resources/Reference Ranges Iron 21042023DP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TrakCareTesting\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PathCare_Projects\TrakCareTesting\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55523BB5-E9EE-433F-BA06-A279CF0B1119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C83370C-0A54-47F3-825A-F937308EE0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0E03FC75-047B-46DB-9414-742DD41215C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E03FC75-047B-46DB-9414-742DD41215C7}"/>
   </bookViews>
   <sheets>
     <sheet name="UserProfile" sheetId="5" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="349">
   <si>
     <t>PK</t>
   </si>
@@ -1093,6 +1093,19 @@
   </si>
   <si>
     <t>specimen receive_FK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+PC.DADC</t>
+  </si>
+  <si>
+    <t>PC Depot Admin and Data Capture PANORAMA</t>
+  </si>
+  <si>
+    <t>Panorama Laboratory</t>
+  </si>
+  <si>
+    <t>PC Lab Assistant PANORAMA</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1229,6 +1242,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1557,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8458A-69AD-496A-81FA-351091BE4C13}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,12 +1993,41 @@
         <v>5</v>
       </c>
     </row>
+    <row r="30" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" t="s">
+        <v>346</v>
+      </c>
+      <c r="D30" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>348</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D30">
     <sortCondition ref="D2:D30"/>
     <sortCondition ref="B2:B30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4066,7 +4111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F1C6DF-1A8D-41A4-9C21-5C5D6D967960}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>